<commit_message>
Agregado filtro de servicio para asistencias generales (se debe corregir para asistencias personales).
</commit_message>
<xml_diff>
--- a/NOAM_ASISTENCIA_V2/Server/wwwroot/docs/NOAM_REPORTES_31.xlsx
+++ b/NOAM_ASISTENCIA_V2/Server/wwwroot/docs/NOAM_REPORTES_31.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROYECTOS\FIME\NOAM_ASISTENCIA_v2\NOAM_ASISTENCIA_V2\Server\wwwroot\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A5A9E6-C3A0-4B4A-A8CD-C83E9AA72BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2672F129-31BC-423E-A5D6-65B3C305471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7A26607A-8AD9-4F9E-A4BC-D55BA9D7932A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$4:$C$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -81,7 +84,7 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -89,7 +92,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -116,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -251,45 +254,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -436,6 +400,48 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -444,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,32 +465,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -496,65 +534,36 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,16 +593,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>624839</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>274320</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>511492</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1376532</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>284145</xdr:rowOff>
+      <xdr:rowOff>320039</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -622,8 +631,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9738360" y="274320"/>
-          <a:ext cx="1898332" cy="642285"/>
+          <a:off x="624839" y="60960"/>
+          <a:ext cx="2207113" cy="746759"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -935,517 +944,519 @@
   <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="8"/>
-    <col min="2" max="2" width="11.5546875" style="4"/>
-    <col min="3" max="3" width="11.5546875" style="32"/>
-    <col min="4" max="4" width="11.5546875" style="39"/>
-    <col min="5" max="5" width="3" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="3" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="3" style="27" customWidth="1"/>
-    <col min="12" max="12" width="2.88671875" style="27" customWidth="1"/>
-    <col min="13" max="13" width="3" style="27" customWidth="1"/>
-    <col min="14" max="34" width="3" style="27" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="3" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.21875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="29.77734375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="2.77734375" style="24" customWidth="1"/>
+    <col min="5" max="5" width="3" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="3" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="3" style="14" customWidth="1"/>
+    <col min="12" max="12" width="2.88671875" style="14" customWidth="1"/>
+    <col min="13" max="13" width="3" style="14" customWidth="1"/>
+    <col min="14" max="34" width="3" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="2" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:35" s="2" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="15"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="35"/>
     </row>
     <row r="2" spans="1:35" s="2" customFormat="1" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="12"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="37"/>
     </row>
     <row r="3" spans="1:35" s="2" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="16" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
-      <c r="AD3" s="17"/>
-      <c r="AE3" s="17"/>
-      <c r="AF3" s="17"/>
-      <c r="AG3" s="17"/>
-      <c r="AH3" s="17"/>
-      <c r="AI3" s="18"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="30"/>
     </row>
     <row r="4" spans="1:35" s="1" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="33">
+      <c r="D4" s="9"/>
+      <c r="E4" s="27">
         <v>1</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="25">
         <v>2</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="25">
         <v>3</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="25">
         <v>4</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="25">
         <v>5</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="25">
         <v>6</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="25">
         <v>7</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="25">
         <v>8</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="25">
         <v>9</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="25">
         <v>10</v>
       </c>
-      <c r="O4" s="9">
+      <c r="O4" s="25">
         <v>11</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="25">
         <v>12</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="Q4" s="25">
         <v>13</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="25">
         <v>14</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="25">
         <v>15</v>
       </c>
-      <c r="T4" s="9">
+      <c r="T4" s="25">
         <v>16</v>
       </c>
-      <c r="U4" s="9">
+      <c r="U4" s="25">
         <v>17</v>
       </c>
-      <c r="V4" s="9">
+      <c r="V4" s="25">
         <v>18</v>
       </c>
-      <c r="W4" s="9">
+      <c r="W4" s="25">
         <v>19</v>
       </c>
-      <c r="X4" s="9">
+      <c r="X4" s="25">
         <v>20</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="Y4" s="25">
         <v>21</v>
       </c>
-      <c r="Z4" s="9">
+      <c r="Z4" s="25">
         <v>22</v>
       </c>
-      <c r="AA4" s="9">
+      <c r="AA4" s="25">
         <v>23</v>
       </c>
-      <c r="AB4" s="9">
+      <c r="AB4" s="25">
         <v>24</v>
       </c>
-      <c r="AC4" s="9">
+      <c r="AC4" s="25">
         <v>25</v>
       </c>
-      <c r="AD4" s="9">
+      <c r="AD4" s="25">
         <v>26</v>
       </c>
-      <c r="AE4" s="9">
+      <c r="AE4" s="25">
         <v>27</v>
       </c>
-      <c r="AF4" s="9">
+      <c r="AF4" s="25">
         <v>28</v>
       </c>
-      <c r="AG4" s="9">
+      <c r="AG4" s="25">
         <v>29</v>
       </c>
-      <c r="AH4" s="9">
+      <c r="AH4" s="25">
         <v>30</v>
       </c>
-      <c r="AI4" s="9">
+      <c r="AI4" s="25">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="24"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="11"/>
     </row>
     <row r="6" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-      <c r="W6" s="25"/>
-      <c r="X6" s="25"/>
-      <c r="Y6" s="25"/>
-      <c r="Z6" s="25"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="25"/>
-      <c r="AC6" s="25"/>
-      <c r="AD6" s="25"/>
-      <c r="AE6" s="25"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="25"/>
-      <c r="AH6" s="25"/>
-      <c r="AI6" s="26"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="13"/>
     </row>
     <row r="7" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
-      <c r="Y7" s="25"/>
-      <c r="Z7" s="25"/>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="25"/>
-      <c r="AC7" s="25"/>
-      <c r="AD7" s="25"/>
-      <c r="AE7" s="25"/>
-      <c r="AF7" s="25"/>
-      <c r="AG7" s="25"/>
-      <c r="AH7" s="25"/>
-      <c r="AI7" s="26"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="12"/>
+      <c r="AI7" s="13"/>
     </row>
     <row r="8" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="25"/>
-      <c r="X8" s="25"/>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="25"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="25"/>
-      <c r="AC8" s="25"/>
-      <c r="AD8" s="25"/>
-      <c r="AE8" s="25"/>
-      <c r="AF8" s="25"/>
-      <c r="AG8" s="25"/>
-      <c r="AH8" s="25"/>
-      <c r="AI8" s="26"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="13"/>
     </row>
     <row r="9" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-      <c r="W9" s="25"/>
-      <c r="X9" s="25"/>
-      <c r="Y9" s="25"/>
-      <c r="Z9" s="25"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="25"/>
-      <c r="AC9" s="25"/>
-      <c r="AD9" s="25"/>
-      <c r="AE9" s="25"/>
-      <c r="AF9" s="25"/>
-      <c r="AG9" s="25"/>
-      <c r="AH9" s="25"/>
-      <c r="AI9" s="26"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="12"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="12"/>
+      <c r="AI9" s="13"/>
     </row>
     <row r="10" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="3"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-      <c r="W10" s="25"/>
-      <c r="X10" s="25"/>
-      <c r="Y10" s="25"/>
-      <c r="Z10" s="25"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="25"/>
-      <c r="AC10" s="25"/>
-      <c r="AD10" s="25"/>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
-      <c r="AH10" s="25"/>
-      <c r="AI10" s="26"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" s="12"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="13"/>
     </row>
     <row r="11" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
-      <c r="AD11" s="25"/>
-      <c r="AE11" s="25"/>
-      <c r="AF11" s="25"/>
-      <c r="AG11" s="25"/>
-      <c r="AH11" s="25"/>
-      <c r="AI11" s="26"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:AI2"/>
-    <mergeCell ref="A1:AI1"/>
+  <autoFilter ref="A4:C11" xr:uid="{F6B9F883-765B-4AC3-9155-BEA24AA6D9C4}"/>
+  <mergeCells count="5">
     <mergeCell ref="E3:AI3"/>
-    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="C1:AI1"/>
+    <mergeCell ref="C2:AI2"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="E1:AI1048576">
+  <conditionalFormatting sqref="E3:AI1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",E1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("F",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>